<commit_message>
Atualização Documento de SharedDimension
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Dominio_SDS.xlsx
+++ b/Documentação/Planilhas/Dominio_SDS.xlsx
@@ -10,15 +10,14 @@
     <sheet name="Dominios SDS " sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Dominios SDS '!$A$1:$F$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Dominios SDS '!$A$1:$F$89</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="194">
   <si>
     <t>stg_cfop.dtsx</t>
   </si>
@@ -546,6 +545,60 @@
   </si>
   <si>
     <t>dw_estoque_loja.dtsx</t>
+  </si>
+  <si>
+    <t>stg_sku_ruptura_vitrine.dtsx</t>
+  </si>
+  <si>
+    <t>Ruptura Vitrine</t>
+  </si>
+  <si>
+    <t>stg_ruptura.dtsx</t>
+  </si>
+  <si>
+    <t>LOJACORP</t>
+  </si>
+  <si>
+    <t>dbo. spETL_source_Sku</t>
+  </si>
+  <si>
+    <t>dbo.stg_corp_sku</t>
+  </si>
+  <si>
+    <t>stg_produto_ruptura_vitrine.dtsx</t>
+  </si>
+  <si>
+    <t>dbo.stg_corp_product</t>
+  </si>
+  <si>
+    <t>dbo.spETL_source_Produto</t>
+  </si>
+  <si>
+    <t>dbo.stg_corp_categoria</t>
+  </si>
+  <si>
+    <t>stg_categoria_ruptura_vitrine.dtsx</t>
+  </si>
+  <si>
+    <t>stg_corp_kit</t>
+  </si>
+  <si>
+    <t>stg_kit_ruptura_vitrine.dtsx</t>
+  </si>
+  <si>
+    <t>dbo.spETL_source_Categoria</t>
+  </si>
+  <si>
+    <t>dbo.spETL_source_SkuKit</t>
+  </si>
+  <si>
+    <t>stg_loja_product</t>
+  </si>
+  <si>
+    <t>stg_product_ruptura_vitrine.dtsx</t>
+  </si>
+  <si>
+    <t>dbo.Produto</t>
   </si>
 </sst>
 </file>
@@ -641,8 +694,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G84" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:G84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G89" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G89">
     <filterColumn colId="6"/>
   </autoFilter>
   <sortState ref="A2:F81">
@@ -946,13 +999,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="16" topLeftCell="E77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -963,7 +1016,7 @@
     <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2656,6 +2709,121 @@
       </c>
       <c r="G84" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>